<commit_message>
one potential way to go. Lots of randomness involved tho
</commit_message>
<xml_diff>
--- a/Tabasco Completes.xlsx
+++ b/Tabasco Completes.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Tabasco" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +15,169 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="108">
+  <si>
+    <t>Adrian</t>
+  </si>
+  <si>
+    <t>Becerra Palos</t>
+  </si>
+  <si>
+    <t>adrianbecerra251@gmail.com</t>
+  </si>
+  <si>
+    <t>Aguascalientes</t>
+  </si>
+  <si>
+    <t>Maria Alejandra</t>
+  </si>
+  <si>
+    <t>Diaz de Leon Macias</t>
+  </si>
+  <si>
+    <t>alejandra.diaz@aguascalientes.gob.mx</t>
+  </si>
+  <si>
+    <t>Jorge</t>
+  </si>
+  <si>
+    <t>Guerra Jimenez</t>
+  </si>
+  <si>
+    <t>asesoria_e@hotmail.com</t>
+  </si>
+  <si>
+    <t>Madeley</t>
+  </si>
+  <si>
+    <t>Rangel Macedonio</t>
+  </si>
+  <si>
+    <t>betyboopmade@hotmail.com</t>
+  </si>
+  <si>
+    <t>Carlos Ernesto</t>
+  </si>
+  <si>
+    <t>MORENO RIVERA</t>
+  </si>
+  <si>
+    <t>cemoreno28@hotmail.com</t>
+  </si>
+  <si>
+    <t>Rigobert</t>
+  </si>
+  <si>
+    <t>Valdez martin del campo</t>
+  </si>
+  <si>
+    <t>estatalpolicia@yahoo.com.mx</t>
+  </si>
+  <si>
+    <t>Juan Eduardo</t>
+  </si>
+  <si>
+    <t>Silva Reyes</t>
+  </si>
+  <si>
+    <t>Gallolalo3621@outlook.es</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Colorado Morales</t>
+  </si>
+  <si>
+    <t>jack01mayo@gmail.com</t>
+  </si>
+  <si>
+    <t>Jose de Jesus</t>
+  </si>
+  <si>
+    <t>Martinez Herrera</t>
+  </si>
+  <si>
+    <t>jesusmherreraoficial@hotmail.com</t>
+  </si>
+  <si>
+    <t>Jose Manuel</t>
+  </si>
+  <si>
+    <t>Soto Guzman</t>
+  </si>
+  <si>
+    <t>josesoto1loky@gmail.com</t>
+  </si>
+  <si>
+    <t>Guillermo</t>
+  </si>
+  <si>
+    <t>De la Paz Ortega</t>
+  </si>
+  <si>
+    <t>kpaz1980logan@gmail.com</t>
+  </si>
+  <si>
+    <t>Lucila</t>
+  </si>
+  <si>
+    <t>Vela Lopez</t>
+  </si>
+  <si>
+    <t>luci.ju.al.03@gmail.com</t>
+  </si>
+  <si>
+    <t>Maria Guadalupe</t>
+  </si>
+  <si>
+    <t>Romo Padilla</t>
+  </si>
+  <si>
+    <t>lupitaromo_2012@hotmail.com</t>
+  </si>
+  <si>
+    <t>Miguel</t>
+  </si>
+  <si>
+    <t>Vazquez Cervantes</t>
+  </si>
+  <si>
+    <t>maria.flore@aguascalientes.gob.mx</t>
+  </si>
+  <si>
+    <t>Norma Angelica</t>
+  </si>
+  <si>
+    <t>Chacon Estrada</t>
+  </si>
+  <si>
+    <t>n-chacon@hotmail.com</t>
+  </si>
+  <si>
+    <t>Jose Alfredo</t>
+  </si>
+  <si>
+    <t>Vital Silva</t>
+  </si>
+  <si>
+    <t>vitaljosealfredo@gmail.com</t>
+  </si>
+  <si>
+    <t>Waldemar</t>
+  </si>
+  <si>
+    <t>waldemarc_ags@yahoo.com.mx</t>
+  </si>
+  <si>
+    <t>Wendy Fabiola</t>
+  </si>
+  <si>
+    <t>Almanza Rodriguez</t>
+  </si>
+  <si>
+    <t>wendy.almanza@aguascalientes.gob.mx</t>
+  </si>
   <si>
     <t>Evelio</t>
   </si>
@@ -26,7 +188,7 @@
     <t>balcazar_perez@hotmail.com</t>
   </si>
   <si>
-    <t>Secretaría de Seguridad Pública del Estado de Tabasco</t>
+    <t>Tabasco</t>
   </si>
   <si>
     <t>Cándido</t>
@@ -117,9 +279,6 @@
   </si>
   <si>
     <t>rafacolladog20@gmail.com</t>
-  </si>
-  <si>
-    <t>Secretaría de Seguridad Pública de Tabasco</t>
   </si>
   <si>
     <t>Rene</t>
@@ -515,7 +674,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,258 +682,542 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="n">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="n">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" t="n">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="n">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="n">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="n">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="n">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="n">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" t="n">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" t="n">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" t="n">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" t="n">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" t="n">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" t="n">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" t="n">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" t="n">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" t="s">
-        <v>3</v>
-      </c>
-    </row>
+    </row>
+    <row r="19" spans="1:5"/>
+    <row r="20" spans="1:5"/>
+    <row r="21" spans="1:5"/>
+    <row r="22" spans="1:5"/>
+    <row r="23" spans="1:5"/>
+    <row r="24" spans="1:5"/>
+    <row r="25" spans="1:5"/>
+    <row r="26" spans="1:5"/>
+    <row r="27" spans="1:5"/>
+    <row r="28" spans="1:5"/>
+    <row r="29" spans="1:5"/>
+    <row r="30" spans="1:5"/>
+    <row r="31" spans="1:5"/>
+    <row r="32" spans="1:5"/>
+    <row r="33" spans="1:5"/>
+    <row r="34" spans="1:5"/>
+    <row r="35" spans="1:5"/>
+    <row r="36" spans="1:5"/>
+    <row r="37" spans="1:5"/>
+    <row r="38" spans="1:5"/>
+    <row r="39" spans="1:5"/>
+    <row r="40" spans="1:5"/>
+    <row r="41" spans="1:5"/>
+    <row r="42" spans="1:5"/>
+    <row r="43" spans="1:5"/>
+    <row r="44" spans="1:5"/>
+    <row r="45" spans="1:5"/>
+    <row r="46" spans="1:5"/>
+    <row r="47" spans="1:5"/>
+    <row r="48" spans="1:5"/>
+    <row r="49" spans="1:5"/>
+    <row r="50" spans="1:5"/>
+    <row r="51" spans="1:5"/>
+    <row r="52" spans="1:5"/>
+    <row r="53" spans="1:5"/>
+    <row r="54" spans="1:5"/>
+    <row r="55" spans="1:5"/>
+    <row r="56" spans="1:5"/>
+    <row r="57" spans="1:5"/>
+    <row r="58" spans="1:5"/>
+    <row r="59" spans="1:5"/>
+    <row r="60" spans="1:5"/>
+    <row r="61" spans="1:5"/>
+    <row r="62" spans="1:5"/>
+    <row r="63" spans="1:5"/>
+    <row r="64" spans="1:5"/>
+    <row r="65" spans="1:5"/>
+    <row r="66" spans="1:5"/>
+    <row r="67" spans="1:5"/>
+    <row r="68" spans="1:5"/>
+    <row r="69" spans="1:5"/>
+    <row r="70" spans="1:5"/>
+    <row r="71" spans="1:5"/>
+    <row r="72" spans="1:5"/>
+    <row r="73" spans="1:5"/>
+    <row r="74" spans="1:5"/>
+    <row r="75" spans="1:5"/>
+    <row r="76" spans="1:5"/>
+    <row r="77" spans="1:5"/>
+    <row r="78" spans="1:5"/>
+    <row r="79" spans="1:5"/>
+    <row r="80" spans="1:5"/>
+    <row r="81" spans="1:5"/>
+    <row r="82" spans="1:5"/>
+    <row r="83" spans="1:5"/>
+    <row r="84" spans="1:5"/>
+    <row r="85" spans="1:5"/>
+    <row r="86" spans="1:5"/>
+    <row r="87" spans="1:5"/>
+    <row r="88" spans="1:5"/>
+    <row r="89" spans="1:5"/>
+    <row r="90" spans="1:5"/>
+    <row r="91" spans="1:5"/>
+    <row r="92" spans="1:5"/>
+    <row r="93" spans="1:5"/>
+    <row r="94" spans="1:5"/>
+    <row r="95" spans="1:5"/>
+    <row r="96" spans="1:5"/>
+    <row r="97" spans="1:5"/>
+    <row r="98" spans="1:5"/>
+    <row r="99" spans="1:5"/>
+    <row r="100" spans="1:5"/>
+    <row r="101" spans="1:5"/>
+    <row r="102" spans="1:5"/>
+    <row r="103" spans="1:5"/>
+    <row r="104" spans="1:5"/>
+    <row r="105" spans="1:5"/>
+    <row r="106" spans="1:5"/>
+    <row r="107" spans="1:5"/>
+    <row r="108" spans="1:5"/>
+    <row r="109" spans="1:5"/>
+    <row r="110" spans="1:5"/>
+    <row r="111" spans="1:5"/>
+    <row r="112" spans="1:5"/>
+    <row r="113" spans="1:5"/>
+    <row r="114" spans="1:5"/>
+    <row r="115" spans="1:5"/>
+    <row r="116" spans="1:5"/>
+    <row r="117" spans="1:5"/>
+    <row r="118" spans="1:5"/>
+    <row r="119" spans="1:5"/>
+    <row r="120" spans="1:5"/>
+    <row r="121" spans="1:5"/>
+    <row r="122" spans="1:5"/>
+    <row r="123" spans="1:5"/>
+    <row r="124" spans="1:5"/>
+    <row r="125" spans="1:5"/>
+    <row r="126" spans="1:5"/>
+    <row r="127" spans="1:5"/>
+    <row r="128" spans="1:5"/>
+    <row r="129" spans="1:5"/>
+    <row r="130" spans="1:5"/>
+    <row r="131" spans="1:5"/>
+    <row r="132" spans="1:5"/>
+    <row r="133" spans="1:5"/>
+    <row r="134" spans="1:5"/>
+    <row r="135" spans="1:5"/>
+    <row r="136" spans="1:5"/>
+    <row r="137" spans="1:5"/>
+    <row r="138" spans="1:5"/>
+    <row r="139" spans="1:5"/>
+    <row r="140" spans="1:5"/>
+    <row r="141" spans="1:5"/>
+    <row r="142" spans="1:5"/>
+    <row r="143" spans="1:5"/>
+    <row r="144" spans="1:5"/>
+    <row r="145" spans="1:5"/>
+    <row r="146" spans="1:5"/>
+    <row r="147" spans="1:5"/>
+    <row r="148" spans="1:5"/>
+    <row r="149" spans="1:5"/>
+    <row r="150" spans="1:5"/>
+    <row r="151" spans="1:5"/>
+    <row r="152" spans="1:5"/>
+    <row r="153" spans="1:5"/>
+    <row r="154" spans="1:5"/>
+    <row r="155" spans="1:5"/>
+    <row r="156" spans="1:5"/>
+    <row r="157" spans="1:5"/>
+    <row r="158" spans="1:5"/>
+    <row r="159" spans="1:5"/>
+    <row r="160" spans="1:5"/>
+    <row r="161" spans="1:5"/>
+    <row r="162" spans="1:5"/>
+    <row r="163" spans="1:5"/>
+    <row r="164" spans="1:5"/>
+    <row r="165" spans="1:5"/>
+    <row r="166" spans="1:5"/>
+    <row r="167" spans="1:5"/>
+    <row r="168" spans="1:5"/>
+    <row r="169" spans="1:5"/>
+    <row r="170" spans="1:5"/>
+    <row r="171" spans="1:5"/>
+    <row r="172" spans="1:5"/>
+    <row r="173" spans="1:5"/>
+    <row r="174" spans="1:5"/>
+    <row r="175" spans="1:5"/>
+    <row r="176" spans="1:5"/>
+    <row r="177" spans="1:5"/>
+    <row r="178" spans="1:5"/>
+    <row r="179" spans="1:5"/>
+    <row r="180" spans="1:5"/>
+    <row r="181" spans="1:5"/>
+    <row r="182" spans="1:5"/>
+    <row r="183" spans="1:5"/>
+    <row r="184" spans="1:5"/>
+    <row r="185" spans="1:5"/>
+    <row r="186" spans="1:5"/>
+    <row r="187" spans="1:5"/>
+    <row r="188" spans="1:5"/>
+    <row r="189" spans="1:5"/>
+    <row r="190" spans="1:5"/>
+    <row r="191" spans="1:5"/>
+    <row r="192" spans="1:5"/>
+    <row r="193" spans="1:5"/>
+    <row r="194" spans="1:5"/>
+    <row r="195" spans="1:5"/>
+    <row r="196" spans="1:5"/>
+    <row r="197" spans="1:5"/>
+    <row r="198" spans="1:5"/>
+    <row r="199" spans="1:5"/>
+    <row r="200" spans="1:5"/>
+    <row r="201" spans="1:5"/>
+    <row r="202" spans="1:5"/>
+    <row r="203" spans="1:5"/>
+    <row r="204" spans="1:5"/>
+    <row r="205" spans="1:5"/>
+    <row r="206" spans="1:5"/>
+    <row r="207" spans="1:5"/>
+    <row r="208" spans="1:5"/>
+    <row r="209" spans="1:5"/>
+    <row r="210" spans="1:5"/>
+    <row r="211" spans="1:5"/>
+    <row r="212" spans="1:5"/>
+    <row r="213" spans="1:5"/>
+    <row r="214" spans="1:5"/>
+    <row r="215" spans="1:5"/>
+    <row r="216" spans="1:5"/>
+    <row r="217" spans="1:5"/>
+    <row r="218" spans="1:5"/>
+    <row r="219" spans="1:5"/>
+    <row r="220" spans="1:5"/>
+    <row r="221" spans="1:5"/>
+    <row r="222" spans="1:5"/>
+    <row r="223" spans="1:5"/>
+    <row r="224" spans="1:5"/>
+    <row r="225" spans="1:5"/>
+    <row r="226" spans="1:5"/>
+    <row r="227" spans="1:5"/>
+    <row r="228" spans="1:5"/>
+    <row r="229" spans="1:5"/>
+    <row r="230" spans="1:5"/>
+    <row r="231" spans="1:5"/>
+    <row r="232" spans="1:5"/>
+    <row r="233" spans="1:5"/>
+    <row r="234" spans="1:5"/>
+    <row r="235" spans="1:5"/>
+    <row r="236" spans="1:5"/>
+    <row r="237" spans="1:5"/>
+    <row r="238" spans="1:5"/>
+    <row r="239" spans="1:5"/>
+    <row r="240" spans="1:5"/>
+    <row r="241" spans="1:5"/>
+    <row r="242" spans="1:5"/>
+    <row r="243" spans="1:5"/>
+    <row r="244" spans="1:5"/>
+    <row r="245" spans="1:5"/>
+    <row r="246" spans="1:5"/>
+    <row r="247" spans="1:5"/>
+    <row r="248" spans="1:5"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>